<commit_message>
lock (bug!) en removeTab
</commit_message>
<xml_diff>
--- a/public/cohort/fileExcel/_sjabloon_v2.xlsx
+++ b/public/cohort/fileExcel/_sjabloon_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csgnl-my.sharepoint.com/personal/vnr_csg_nl/Documents/SCHOOLdocumenten/CORONA/PTO PTA/cohortproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="310" documentId="11_AD4D7A0C205A6B9A452FA84F5F1974425ADEDD8A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{42141C40-5B1A-478C-93EB-46F6E3AD332D}"/>
+  <xr:revisionPtr revIDLastSave="324" documentId="11_AD4D7A0C205A6B9A452FA84F5F1974425ADEDD8A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{91636D34-FF9C-4D28-93B8-9ADFA081BE08}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="59">
   <si>
     <t>statusCode</t>
   </si>
@@ -195,6 +195,15 @@
   </si>
   <si>
     <t>mavo?</t>
+  </si>
+  <si>
+    <t>niet formatten. Layouten doen wij.</t>
+  </si>
+  <si>
+    <t>zie je iets waarvan je denkt dat het niet klopt! Mail me.</t>
+  </si>
+  <si>
+    <t>niet in oude Excel openen. Op school / in Teams.</t>
   </si>
 </sst>
 </file>
@@ -1310,14 +1319,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:A9"/>
+  <dimension ref="A2:A9"/>
   <sheetViews>
     <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
@@ -1336,6 +1350,16 @@
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -1356,7 +1380,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1420,7 +1444,7 @@
       </c>
       <c r="D4" s="2"/>
       <c r="G4" s="17" t="str">
-        <f>CONCATENATE(B4," leerlaag ",B6,"4 (schooljaar ",B7," - ",B7+1,")")</f>
+        <f>CONCATENATE(B4," leerlaag ",B6,B15," (schooljaar ",B7," - ",B7+1,")")</f>
         <v xml:space="preserve"> leerlaag 4 (schooljaar  - 1)</v>
       </c>
     </row>
@@ -1579,7 +1603,7 @@
       </c>
       <c r="B10" s="6">
         <f ca="1">NOW()</f>
-        <v>44340.533850115738</v>
+        <v>44340.684103703701</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1694,7 +1718,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="G16" s="17" t="str">
-        <f>CONCATENATE(B4," leerlaag ",B6,"5 (schooljaar ",B7+1," - ",B7+2,")")</f>
+        <f>CONCATENATE(B4," leerlaag ",B6,B15+1," (schooljaar ",B7+1," - ",B7+2,")")</f>
         <v xml:space="preserve"> leerlaag 5 (schooljaar 1 - 2)</v>
       </c>
     </row>
@@ -1899,7 +1923,7 @@
       </c>
       <c r="D28" s="2"/>
       <c r="G28" s="17" t="str">
-        <f>CONCATENATE(B4," leerlaag ",B6,"6 (schooljaar ",B7+2," - ",B9,")")</f>
+        <f>CONCATENATE(B4," leerlaag ",B6,B15+2," (schooljaar ",B7+2," - ",B9,")")</f>
         <v xml:space="preserve"> leerlaag 6 (schooljaar 2 - 1)</v>
       </c>
     </row>

</xml_diff>